<commit_message>
update feature Fixed Delay, Log Failed Contact, Pause & Resume, Countdown Timer
</commit_message>
<xml_diff>
--- a/contohdata.xlsx
+++ b/contohdata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Coding\AutoBlast\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{161A404D-DBA4-46D2-9F5C-7395C9ABA6F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{230C0EE4-EC9B-468C-8C75-2D0FBE0B95CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="7">
   <si>
     <t>Nama</t>
   </si>
@@ -38,6 +38,9 @@
   </si>
   <si>
     <t>https://api.whatsapp.com/send?phone=6285111210304&amp;text=Halloo%2C%20kak%20NAUFAL%20IMAM%20HIDAYATULLAH%0AAlumni%20UIN%20Syarif%20Hidayatullah%20Jakarta%0AAngkatan%20Wisuda%20131%0A%0AAssalamualaikum%20Wr.Wb.%20%0ADengan%20hormat%2C%20kami%20tim%20Pusat%20Karier%20UIN%20Jakarta%20mengundang%20Anda%20untuk%20berpartisipasi%20dalam%20penyelenggaraan%20Tracer%20Study%20UIN%20Jakarta%202025%20dengan%20mengisi%20survei%20karier%20alumni%20guna%20membantu%20mengevaluasi%20dan%20meningkatkan%20kualitas%20pendidikan%20UIN%20Syarif%20Hidayatullah%20Jakarta.%0A%20%0ABerikut%20merupakan%20langkah-langkah%20untuk%20berpartisipasi%20dalam%20TS%20UIN%20Jakarta%202025.%0ATutorial%20Pengisian%3A%0A1.%20Buka%20Google%20Form%20TS%20Pusat%20Karier%20UIN%20Jakarta%20dengan%20mengakses%20link%20berikut%3A%20https%3A%2F%2Fs.id%2FTSUINJKT2025%0A2.%20Kemudian%2C%20silahkan%20mengisi%20seluruh%20pertanyaan%20dan%20klik%20%E2%80%98Kirim%27%0A3.%20Jika%20ada%20pertanyaan%2C%20silahkan%20berkabar%20melalui%20chat%20WA%20ini%0A%0AAtas%20perhatian%20dan%20partisipasi%20anda%2C%20kami%20ucapkan%20terima%20kasih.%20Semoga%2C%20keberkahan%20dan%20perlindungan%20Allah%20SWT%20selalu%20menyertai%20perjalanan%20karier%20anda.%0A%0ASalam%20Hangat%0A%28Pusat%20Karier%20UIN%20Jakarta%29%0A%0AMengetahui%0AM.%20Kholis%20Hamdy%0A%0AKepala%20Pusat%20Karier%20UIN%20Jakarta</t>
+  </si>
+  <si>
+    <t>https://api.whatsapp.com/send?phone=6285892254838&amp;text=Halloo%2C%20kak%20NAUFAL%20IMAM%20HIDAYATULLAH%0AAlumni%20UIN%20Syarif%20Hidayatullah%20Jakarta%0AAngkatan%20Wisuda%20131%0A%0AAssalamualaikum%20Wr.Wb.%20%0ADengan%20hormat%2C%20kami%20tim%20Pusat%20Karier%20UIN%20Jakarta%20mengundang%20Anda%20untuk%20berpartisipasi%20dalam%20penyelenggaraan%20Tracer%20Study%20UIN%20Jakarta%202025%20dengan%20mengisi%20survei%20karier%20alumni%20guna%20membantu%20mengevaluasi%20dan%20meningkatkan%20kualitas%20pendidikan%20UIN%20Syarif%20Hidayatullah%20Jakarta.%0A%20%0ABerikut%20merupakan%20langkah-langkah%20untuk%20berpartisipasi%20dalam%20TS%20UIN%20Jakarta%202025.%0ATutorial%20Pengisian%3A%0A1.%20Buka%20Google%20Form%20TS%20Pusat%20Karier%20UIN%20Jakarta%20dengan%20mengakses%20link%20berikut%3A%20https%3A%2F%2Fs.id%2FTSUINJKT2025%0A2.%20Kemudian%2C%20silahkan%20mengisi%20seluruh%20pertanyaan%20dan%20klik%20%E2%80%98Kirim%27%0A3.%20Jika%20ada%20pertanyaan%2C%20silahkan%20berkabar%20melalui%20chat%20WA%20ini%0A%0AAtas%20perhatian%20dan%20partisipasi%20anda%2C%20kami%20ucapkan%20terima%20kasih.%20Semoga%2C%20keberkahan%20dan%20perlindungan%20Allah%20SWT%20selalu%20menyertai%20perjalanan%20karier%20anda.%0A%0ASalam%20Hangat%0A%28Pusat%20Karier%20UIN%20Jakarta%29%0A%0AMengetahui%0AM.%20Kholis%20Hamdy%0A%0AKepala%20Pusat%20Karier%20UIN%20Jakarta</t>
   </si>
 </sst>
 </file>
@@ -73,8 +76,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -377,10 +381,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -400,10 +404,21 @@
       <c r="A2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>